<commit_message>
edits to latex generation
</commit_message>
<xml_diff>
--- a/experiment_results.xlsx
+++ b/experiment_results.xlsx
@@ -14,24 +14,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>num_points_each_iteration</t>
   </si>
   <si>
     <t>random_sampling</t>
-  </si>
-  <si>
-    <t>relative_alpha_error_after_10_iterations</t>
-  </si>
-  <si>
-    <t>relative_alpha_error_after_15_iterations</t>
-  </si>
-  <si>
-    <t>relative_alpha_error_after_1_iteration</t>
-  </si>
-  <si>
-    <t>relative_alpha_error_after_5_iterations</t>
   </si>
   <si>
     <t>relative_alpha_error_after_iteration_1</t>
@@ -41,15 +29,6 @@
   </si>
   <si>
     <t>relative_alpha_error_after_iteration_15</t>
-  </si>
-  <si>
-    <t>relative_alpha_error_after_iteration_20</t>
-  </si>
-  <si>
-    <t>relative_alpha_error_after_iteration_25</t>
-  </si>
-  <si>
-    <t>relative_alpha_error_after_iteration_30</t>
   </si>
   <si>
     <t>relative_alpha_error_after_iteration_5</t>
@@ -410,13 +389,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N17"/>
+  <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:7">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -435,29 +414,8 @@
       <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14">
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -468,40 +426,19 @@
         <v>1</v>
       </c>
       <c r="D2">
-        <v>3.044012606912228</v>
+        <v>2.717047823132128</v>
       </c>
       <c r="E2">
-        <v>2.130937395382903</v>
+        <v>1.294697309447686</v>
       </c>
       <c r="F2">
-        <v>3.216466245049682</v>
+        <v>0.8786615770027312</v>
       </c>
       <c r="G2">
-        <v>3.62264496822141</v>
-      </c>
-      <c r="H2">
-        <v>1</v>
-      </c>
-      <c r="I2">
-        <v>1</v>
-      </c>
-      <c r="J2">
-        <v>1</v>
-      </c>
-      <c r="K2">
-        <v>1</v>
-      </c>
-      <c r="L2">
-        <v>1</v>
-      </c>
-      <c r="M2">
-        <v>1</v>
-      </c>
-      <c r="N2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14">
+        <v>2.389980748059801</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -512,40 +449,19 @@
         <v>1</v>
       </c>
       <c r="D3">
-        <v>0.3309258782030115</v>
+        <v>0.002990230386542744</v>
       </c>
       <c r="E3">
-        <v>0.2345183003469831</v>
+        <v>0.01075151096857592</v>
       </c>
       <c r="F3">
-        <v>2.999602228464676</v>
+        <v>0.002413186324267865</v>
       </c>
       <c r="G3">
-        <v>0.6171263959040454</v>
-      </c>
-      <c r="H3">
-        <v>1</v>
-      </c>
-      <c r="I3">
-        <v>1</v>
-      </c>
-      <c r="J3">
-        <v>1</v>
-      </c>
-      <c r="K3">
-        <v>1</v>
-      </c>
-      <c r="L3">
-        <v>1</v>
-      </c>
-      <c r="M3">
-        <v>1</v>
-      </c>
-      <c r="N3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14">
+        <v>0.006976853060635668</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -556,40 +472,19 @@
         <v>1</v>
       </c>
       <c r="D4">
-        <v>0.01715952240747887</v>
+        <v>0.05938908374888659</v>
       </c>
       <c r="E4">
-        <v>0.01206668888703077</v>
+        <v>0.02977674883433923</v>
       </c>
       <c r="F4">
-        <v>0.003019191485913453</v>
+        <v>0.03086605356512895</v>
       </c>
       <c r="G4">
-        <v>0.037988472957645</v>
-      </c>
-      <c r="H4">
-        <v>1</v>
-      </c>
-      <c r="I4">
-        <v>1</v>
-      </c>
-      <c r="J4">
-        <v>1</v>
-      </c>
-      <c r="K4">
-        <v>1</v>
-      </c>
-      <c r="L4">
-        <v>1</v>
-      </c>
-      <c r="M4">
-        <v>1</v>
-      </c>
-      <c r="N4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14">
+        <v>0.03641558944654621</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -600,40 +495,19 @@
         <v>1</v>
       </c>
       <c r="D5">
-        <v>0.4522684607042003</v>
+        <v>0.02538605013603534</v>
       </c>
       <c r="E5">
-        <v>0.3154538378704121</v>
+        <v>0.01640459566034332</v>
       </c>
       <c r="F5">
-        <v>4.393448314198348</v>
+        <v>0.01916024759184972</v>
       </c>
       <c r="G5">
-        <v>0.867194547100209</v>
-      </c>
-      <c r="H5">
-        <v>1</v>
-      </c>
-      <c r="I5">
-        <v>1</v>
-      </c>
-      <c r="J5">
-        <v>1</v>
-      </c>
-      <c r="K5">
-        <v>1</v>
-      </c>
-      <c r="L5">
-        <v>1</v>
-      </c>
-      <c r="M5">
-        <v>1</v>
-      </c>
-      <c r="N5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14">
+        <v>0.00891768075882482</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -644,40 +518,19 @@
         <v>1</v>
       </c>
       <c r="D6">
-        <v>0.002449663771459758</v>
+        <v>0.001287470726655989</v>
       </c>
       <c r="E6">
-        <v>0.004050794796050343</v>
+        <v>0.02887033941941175</v>
       </c>
       <c r="F6">
-        <v>0.01908844686755858</v>
+        <v>0.02787696376339096</v>
       </c>
       <c r="G6">
-        <v>0.001048577541693704</v>
-      </c>
-      <c r="H6">
-        <v>1</v>
-      </c>
-      <c r="I6">
-        <v>1</v>
-      </c>
-      <c r="J6">
-        <v>1</v>
-      </c>
-      <c r="K6">
-        <v>1</v>
-      </c>
-      <c r="L6">
-        <v>1</v>
-      </c>
-      <c r="M6">
-        <v>1</v>
-      </c>
-      <c r="N6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14">
+        <v>0.02262160853737705</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -688,40 +541,19 @@
         <v>1</v>
       </c>
       <c r="D7">
-        <v>0.04635185796960817</v>
+        <v>0.02333771347491261</v>
       </c>
       <c r="E7">
-        <v>0.03935749562623733</v>
+        <v>0.00717150776429698</v>
       </c>
       <c r="F7">
-        <v>0.02210674305486271</v>
+        <v>0.006828435301917865</v>
       </c>
       <c r="G7">
-        <v>0.06604800655902392</v>
-      </c>
-      <c r="H7">
-        <v>1</v>
-      </c>
-      <c r="I7">
-        <v>1</v>
-      </c>
-      <c r="J7">
-        <v>1</v>
-      </c>
-      <c r="K7">
-        <v>1</v>
-      </c>
-      <c r="L7">
-        <v>1</v>
-      </c>
-      <c r="M7">
-        <v>1</v>
-      </c>
-      <c r="N7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14">
+        <v>0.005400970585088631</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -732,40 +564,19 @@
         <v>1</v>
       </c>
       <c r="D8">
-        <v>0.002119832502906853</v>
+        <v>0.01601261645363968</v>
       </c>
       <c r="E8">
-        <v>0.00262854344740678</v>
+        <v>0.01018788890474964</v>
       </c>
       <c r="F8">
-        <v>0.0113696229431746</v>
+        <v>0.009876392403068517</v>
       </c>
       <c r="G8">
-        <v>0.002406939899718223</v>
-      </c>
-      <c r="H8">
-        <v>1</v>
-      </c>
-      <c r="I8">
-        <v>1</v>
-      </c>
-      <c r="J8">
-        <v>1</v>
-      </c>
-      <c r="K8">
-        <v>1</v>
-      </c>
-      <c r="L8">
-        <v>1</v>
-      </c>
-      <c r="M8">
-        <v>1</v>
-      </c>
-      <c r="N8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14">
+        <v>0.01165205888990495</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -776,40 +587,19 @@
         <v>1</v>
       </c>
       <c r="D9">
-        <v>0.03335534372882198</v>
+        <v>0.01928088929005275</v>
       </c>
       <c r="E9">
-        <v>0.02812819298054529</v>
+        <v>0.01928688441483658</v>
       </c>
       <c r="F9">
-        <v>0.1221912811422852</v>
+        <v>0.01920325312573375</v>
       </c>
       <c r="G9">
-        <v>0.04865223754116077</v>
-      </c>
-      <c r="H9">
-        <v>1</v>
-      </c>
-      <c r="I9">
-        <v>1</v>
-      </c>
-      <c r="J9">
-        <v>1</v>
-      </c>
-      <c r="K9">
-        <v>1</v>
-      </c>
-      <c r="L9">
-        <v>1</v>
-      </c>
-      <c r="M9">
-        <v>1</v>
-      </c>
-      <c r="N9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14">
+        <v>0.0171955972014561</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -820,40 +610,19 @@
         <v>0</v>
       </c>
       <c r="D10">
+        <v>0.3714526161416809</v>
+      </c>
+      <c r="E10">
         <v>0.05598708280918556</v>
       </c>
-      <c r="E10">
+      <c r="F10">
         <v>0.07081928761417482</v>
-      </c>
-      <c r="F10">
-        <v>0.3714526161416809</v>
       </c>
       <c r="G10">
         <v>0.005167383837208125</v>
       </c>
-      <c r="H10">
-        <v>1</v>
-      </c>
-      <c r="I10">
-        <v>1</v>
-      </c>
-      <c r="J10">
-        <v>1</v>
-      </c>
-      <c r="K10">
-        <v>1</v>
-      </c>
-      <c r="L10">
-        <v>1</v>
-      </c>
-      <c r="M10">
-        <v>1</v>
-      </c>
-      <c r="N10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14">
+    </row>
+    <row r="11" spans="1:7">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -864,40 +633,19 @@
         <v>0</v>
       </c>
       <c r="D11">
+        <v>0.1638514317245362</v>
+      </c>
+      <c r="E11">
         <v>0.1037751157421877</v>
       </c>
-      <c r="E11">
+      <c r="F11">
         <v>0.1012359849799753</v>
-      </c>
-      <c r="F11">
-        <v>0.1638514317245362</v>
       </c>
       <c r="G11">
         <v>0.1112472567226847</v>
       </c>
-      <c r="H11">
-        <v>1</v>
-      </c>
-      <c r="I11">
-        <v>1</v>
-      </c>
-      <c r="J11">
-        <v>1</v>
-      </c>
-      <c r="K11">
-        <v>1</v>
-      </c>
-      <c r="L11">
-        <v>1</v>
-      </c>
-      <c r="M11">
-        <v>1</v>
-      </c>
-      <c r="N11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14">
+    </row>
+    <row r="12" spans="1:7">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -908,40 +656,19 @@
         <v>0</v>
       </c>
       <c r="D12">
+        <v>0.1056477568441481</v>
+      </c>
+      <c r="E12">
         <v>0.04926232548982945</v>
       </c>
-      <c r="E12">
+      <c r="F12">
         <v>0.05027155785436221</v>
-      </c>
-      <c r="F12">
-        <v>0.1056477568441481</v>
       </c>
       <c r="G12">
         <v>0.05967054229483423</v>
       </c>
-      <c r="H12">
-        <v>1</v>
-      </c>
-      <c r="I12">
-        <v>1</v>
-      </c>
-      <c r="J12">
-        <v>1</v>
-      </c>
-      <c r="K12">
-        <v>1</v>
-      </c>
-      <c r="L12">
-        <v>1</v>
-      </c>
-      <c r="M12">
-        <v>1</v>
-      </c>
-      <c r="N12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14">
+    </row>
+    <row r="13" spans="1:7">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -952,40 +679,19 @@
         <v>0</v>
       </c>
       <c r="D13">
+        <v>0.1036376959285681</v>
+      </c>
+      <c r="E13">
         <v>0.08164015156627921</v>
       </c>
-      <c r="E13">
+      <c r="F13">
         <v>0.08071131653274666</v>
-      </c>
-      <c r="F13">
-        <v>0.1036376959285681</v>
       </c>
       <c r="G13">
         <v>0.08437757868216193</v>
       </c>
-      <c r="H13">
-        <v>1</v>
-      </c>
-      <c r="I13">
-        <v>1</v>
-      </c>
-      <c r="J13">
-        <v>1</v>
-      </c>
-      <c r="K13">
-        <v>1</v>
-      </c>
-      <c r="L13">
-        <v>1</v>
-      </c>
-      <c r="M13">
-        <v>1</v>
-      </c>
-      <c r="N13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14">
+    </row>
+    <row r="14" spans="1:7">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -996,40 +702,19 @@
         <v>0</v>
       </c>
       <c r="D14">
+        <v>0.08332152410215898</v>
+      </c>
+      <c r="E14">
         <v>0.04521734202520741</v>
       </c>
-      <c r="E14">
+      <c r="F14">
         <v>0.04369464179066307</v>
-      </c>
-      <c r="F14">
-        <v>0.08332152410215898</v>
       </c>
       <c r="G14">
         <v>0.04994229837770425</v>
       </c>
-      <c r="H14">
-        <v>1</v>
-      </c>
-      <c r="I14">
-        <v>1</v>
-      </c>
-      <c r="J14">
-        <v>1</v>
-      </c>
-      <c r="K14">
-        <v>1</v>
-      </c>
-      <c r="L14">
-        <v>1</v>
-      </c>
-      <c r="M14">
-        <v>1</v>
-      </c>
-      <c r="N14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14">
+    </row>
+    <row r="15" spans="1:7">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -1040,40 +725,19 @@
         <v>0</v>
       </c>
       <c r="D15">
+        <v>0.0422178801500489</v>
+      </c>
+      <c r="E15">
         <v>0.03985682015332189</v>
       </c>
-      <c r="E15">
+      <c r="F15">
         <v>0.04062836719702793</v>
-      </c>
-      <c r="F15">
-        <v>0.0422178801500489</v>
       </c>
       <c r="G15">
         <v>0.04140393459587999</v>
       </c>
-      <c r="H15">
-        <v>1</v>
-      </c>
-      <c r="I15">
-        <v>1</v>
-      </c>
-      <c r="J15">
-        <v>1</v>
-      </c>
-      <c r="K15">
-        <v>1</v>
-      </c>
-      <c r="L15">
-        <v>1</v>
-      </c>
-      <c r="M15">
-        <v>1</v>
-      </c>
-      <c r="N15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14">
+    </row>
+    <row r="16" spans="1:7">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -1084,40 +748,19 @@
         <v>0</v>
       </c>
       <c r="D16">
+        <v>0.03112076637644179</v>
+      </c>
+      <c r="E16">
         <v>0.04964217664542155</v>
       </c>
-      <c r="E16">
+      <c r="F16">
         <v>0.05019881740540207</v>
-      </c>
-      <c r="F16">
-        <v>0.03112076637644179</v>
       </c>
       <c r="G16">
         <v>0.04677496815646387</v>
       </c>
-      <c r="H16">
-        <v>1</v>
-      </c>
-      <c r="I16">
-        <v>1</v>
-      </c>
-      <c r="J16">
-        <v>1</v>
-      </c>
-      <c r="K16">
-        <v>1</v>
-      </c>
-      <c r="L16">
-        <v>1</v>
-      </c>
-      <c r="M16">
-        <v>1</v>
-      </c>
-      <c r="N16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:14">
+    </row>
+    <row r="17" spans="1:7">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -1128,37 +771,16 @@
         <v>0</v>
       </c>
       <c r="D17">
+        <v>0.04208760657302209</v>
+      </c>
+      <c r="E17">
         <v>0.03703893368821247</v>
       </c>
-      <c r="E17">
+      <c r="F17">
         <v>0.03668520634206696</v>
-      </c>
-      <c r="F17">
-        <v>0.04208760657302209</v>
       </c>
       <c r="G17">
         <v>0.03968397623199431</v>
-      </c>
-      <c r="H17">
-        <v>1</v>
-      </c>
-      <c r="I17">
-        <v>1</v>
-      </c>
-      <c r="J17">
-        <v>1</v>
-      </c>
-      <c r="K17">
-        <v>1</v>
-      </c>
-      <c r="L17">
-        <v>1</v>
-      </c>
-      <c r="M17">
-        <v>1</v>
-      </c>
-      <c r="N17">
-        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>